<commit_message>
add iteration 2 final edit
</commit_message>
<xml_diff>
--- a/Documents/Iteration Estimated Effort-Iteration2.xlsx
+++ b/Documents/Iteration Estimated Effort-Iteration2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
   <si>
     <t>Task Name: (Dependencies top to bottom)</t>
   </si>
@@ -132,7 +132,28 @@
     <t>Edit Home Page (RV)</t>
   </si>
   <si>
+    <t>Edit Info Page (RV)</t>
+  </si>
+  <si>
     <t>Iteration 3:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystal </t>
+  </si>
+  <si>
+    <t>Design Cards Components</t>
+  </si>
+  <si>
+    <t>Design Carousel component</t>
+  </si>
+  <si>
+    <t>Design Contact Us</t>
+  </si>
+  <si>
+    <t>Design Prices</t>
+  </si>
+  <si>
+    <t>Improve SEO (RV)</t>
   </si>
 </sst>
 </file>
@@ -142,7 +163,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -188,13 +209,22 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
       <sz val="10.0"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +247,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
     <fill>
@@ -366,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="169">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -709,6 +745,15 @@
     <xf borderId="10" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="10" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="12" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -727,14 +772,20 @@
     <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="9" fillId="2" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="9" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -743,10 +794,10 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="2" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -760,26 +811,53 @@
     <xf borderId="1" fillId="4" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="10" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="11" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="11" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="4" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -793,6 +871,9 @@
     <xf borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -805,22 +886,22 @@
     <xf borderId="5" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="9" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="6" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2585,7 +2666,7 @@
       <c r="M36" s="113"/>
       <c r="N36" s="113"/>
       <c r="O36" s="113"/>
-      <c r="P36" s="113"/>
+      <c r="P36" s="114"/>
       <c r="Q36" s="113">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2619,7 +2700,9 @@
       <c r="F37" s="44">
         <v>1.0</v>
       </c>
-      <c r="G37" s="112"/>
+      <c r="G37" s="115">
+        <v>1.0</v>
+      </c>
       <c r="H37" s="52"/>
       <c r="I37" s="112"/>
       <c r="J37" s="4"/>
@@ -2627,11 +2710,13 @@
       <c r="L37" s="4"/>
       <c r="M37" s="113"/>
       <c r="N37" s="113"/>
-      <c r="O37" s="113"/>
-      <c r="P37" s="113"/>
+      <c r="O37" s="116">
+        <v>1.0</v>
+      </c>
+      <c r="P37" s="114"/>
       <c r="Q37" s="113">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
@@ -2671,7 +2756,7 @@
       <c r="M38" s="113"/>
       <c r="N38" s="113"/>
       <c r="O38" s="113"/>
-      <c r="P38" s="113"/>
+      <c r="P38" s="114"/>
       <c r="Q38" s="113">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2705,7 +2790,9 @@
       <c r="F39" s="44">
         <v>2.0</v>
       </c>
-      <c r="G39" s="112"/>
+      <c r="G39" s="115">
+        <v>1.0</v>
+      </c>
       <c r="H39" s="52"/>
       <c r="I39" s="112"/>
       <c r="J39" s="4"/>
@@ -2713,11 +2800,13 @@
       <c r="L39" s="4"/>
       <c r="M39" s="113"/>
       <c r="N39" s="113"/>
-      <c r="O39" s="113"/>
-      <c r="P39" s="113"/>
+      <c r="O39" s="116">
+        <v>1.0</v>
+      </c>
+      <c r="P39" s="114"/>
       <c r="Q39" s="113">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R39" s="4"/>
       <c r="S39" s="4"/>
@@ -2737,28 +2826,28 @@
     </row>
     <row r="40">
       <c r="A40" s="107"/>
-      <c r="B40" s="114" t="s">
+      <c r="B40" s="117" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="58"/>
       <c r="D40" s="59"/>
-      <c r="E40" s="115" t="s">
+      <c r="E40" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="116">
+      <c r="F40" s="119">
         <v>2.0</v>
       </c>
-      <c r="G40" s="117"/>
+      <c r="G40" s="120"/>
       <c r="H40" s="61"/>
-      <c r="I40" s="117"/>
+      <c r="I40" s="120"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="118"/>
-      <c r="N40" s="118"/>
-      <c r="O40" s="118"/>
-      <c r="P40" s="118"/>
-      <c r="Q40" s="118">
+      <c r="M40" s="121"/>
+      <c r="N40" s="121"/>
+      <c r="O40" s="121"/>
+      <c r="P40" s="121"/>
+      <c r="Q40" s="121">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2788,12 +2877,12 @@
       <c r="E41" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="119">
+      <c r="F41" s="122">
         <v>1.0</v>
       </c>
       <c r="G41" s="109">
         <f>SUM(F42:F46)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H41" s="105"/>
       <c r="I41" s="109">
@@ -2805,11 +2894,13 @@
       <c r="L41" s="4"/>
       <c r="M41" s="110"/>
       <c r="N41" s="110"/>
-      <c r="O41" s="110"/>
-      <c r="P41" s="110"/>
+      <c r="O41" s="123"/>
+      <c r="P41" s="124">
+        <v>10.0</v>
+      </c>
       <c r="Q41" s="110">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R41" s="4"/>
       <c r="S41" s="4"/>
@@ -2849,10 +2940,12 @@
       <c r="M42" s="113"/>
       <c r="N42" s="113"/>
       <c r="O42" s="113"/>
-      <c r="P42" s="113"/>
+      <c r="P42" s="114">
+        <v>2.0</v>
+      </c>
       <c r="Q42" s="113">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
@@ -2954,11 +3047,17 @@
     </row>
     <row r="45">
       <c r="A45" s="107"/>
-      <c r="B45" s="120"/>
+      <c r="B45" s="111" t="s">
+        <v>38</v>
+      </c>
       <c r="C45" s="41"/>
       <c r="D45" s="42"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="52"/>
+      <c r="E45" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="44">
+        <v>3.0</v>
+      </c>
       <c r="G45" s="112"/>
       <c r="H45" s="52"/>
       <c r="I45" s="112"/>
@@ -2968,10 +3067,12 @@
       <c r="M45" s="113"/>
       <c r="N45" s="113"/>
       <c r="O45" s="113"/>
-      <c r="P45" s="113"/>
+      <c r="P45" s="114">
+        <v>4.0</v>
+      </c>
       <c r="Q45" s="113">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R45" s="4"/>
       <c r="S45" s="4"/>
@@ -2991,22 +3092,22 @@
     </row>
     <row r="46">
       <c r="A46" s="107"/>
-      <c r="B46" s="121"/>
+      <c r="B46" s="125"/>
       <c r="C46" s="58"/>
       <c r="D46" s="59"/>
       <c r="E46" s="60"/>
       <c r="F46" s="61"/>
-      <c r="G46" s="117"/>
+      <c r="G46" s="120"/>
       <c r="H46" s="61"/>
-      <c r="I46" s="117"/>
+      <c r="I46" s="120"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
-      <c r="M46" s="118"/>
-      <c r="N46" s="118"/>
-      <c r="O46" s="118"/>
-      <c r="P46" s="118"/>
-      <c r="Q46" s="118">
+      <c r="M46" s="121"/>
+      <c r="N46" s="121"/>
+      <c r="O46" s="121"/>
+      <c r="P46" s="121"/>
+      <c r="Q46" s="121">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3031,7 +3132,7 @@
       <c r="B47" s="54"/>
       <c r="C47" s="108"/>
       <c r="D47" s="76"/>
-      <c r="E47" s="122"/>
+      <c r="E47" s="126"/>
       <c r="F47" s="105"/>
       <c r="G47" s="109">
         <f>SUM(F48:F50)</f>
@@ -3071,7 +3172,7 @@
     </row>
     <row r="48">
       <c r="A48" s="107"/>
-      <c r="B48" s="120"/>
+      <c r="B48" s="127"/>
       <c r="C48" s="41"/>
       <c r="D48" s="42"/>
       <c r="E48" s="51"/>
@@ -3108,10 +3209,10 @@
     </row>
     <row r="49">
       <c r="A49" s="107"/>
-      <c r="B49" s="120"/>
+      <c r="B49" s="127"/>
       <c r="C49" s="41"/>
       <c r="D49" s="42"/>
-      <c r="E49" s="123"/>
+      <c r="E49" s="128"/>
       <c r="F49" s="52"/>
       <c r="G49" s="112"/>
       <c r="H49" s="52"/>
@@ -3145,22 +3246,22 @@
     </row>
     <row r="50">
       <c r="A50" s="107"/>
-      <c r="B50" s="121"/>
+      <c r="B50" s="125"/>
       <c r="C50" s="58"/>
       <c r="D50" s="59"/>
       <c r="E50" s="60"/>
       <c r="F50" s="61"/>
-      <c r="G50" s="117"/>
+      <c r="G50" s="120"/>
       <c r="H50" s="61"/>
-      <c r="I50" s="117"/>
+      <c r="I50" s="120"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
-      <c r="M50" s="118"/>
-      <c r="N50" s="118"/>
-      <c r="O50" s="118"/>
-      <c r="P50" s="118"/>
-      <c r="Q50" s="118">
+      <c r="M50" s="121"/>
+      <c r="N50" s="121"/>
+      <c r="O50" s="121"/>
+      <c r="P50" s="121"/>
+      <c r="Q50" s="121">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3182,16 +3283,22 @@
     </row>
     <row r="51">
       <c r="A51" s="74" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
-      <c r="B51" s="54"/>
+      <c r="B51" s="32" t="s">
+        <v>28</v>
+      </c>
       <c r="C51" s="108"/>
       <c r="D51" s="76"/>
-      <c r="E51" s="122"/>
-      <c r="F51" s="79"/>
+      <c r="E51" s="77" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51" s="78">
+        <v>6.0</v>
+      </c>
       <c r="G51" s="109">
         <f>SUM(F52:F55)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H51" s="79"/>
       <c r="I51" s="109">
@@ -3226,23 +3333,27 @@
       <c r="AF51" s="5"/>
     </row>
     <row r="52">
-      <c r="A52" s="124"/>
-      <c r="B52" s="125"/>
+      <c r="A52" s="129"/>
+      <c r="B52" s="130" t="s">
+        <v>41</v>
+      </c>
       <c r="C52" s="66"/>
       <c r="D52" s="67"/>
-      <c r="E52" s="126"/>
-      <c r="F52" s="127"/>
-      <c r="G52" s="128"/>
-      <c r="H52" s="127"/>
-      <c r="I52" s="129"/>
+      <c r="E52" s="131" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="132"/>
+      <c r="G52" s="133"/>
+      <c r="H52" s="132"/>
+      <c r="I52" s="134"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="130"/>
-      <c r="N52" s="130"/>
-      <c r="O52" s="130"/>
-      <c r="P52" s="130"/>
-      <c r="Q52" s="130">
+      <c r="M52" s="135"/>
+      <c r="N52" s="135"/>
+      <c r="O52" s="135"/>
+      <c r="P52" s="135"/>
+      <c r="Q52" s="135">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3264,13 +3375,19 @@
     </row>
     <row r="53">
       <c r="A53" s="74"/>
-      <c r="B53" s="95"/>
+      <c r="B53" s="136" t="s">
+        <v>42</v>
+      </c>
       <c r="C53" s="94"/>
       <c r="D53" s="83"/>
-      <c r="E53" s="131"/>
-      <c r="F53" s="132"/>
+      <c r="E53" s="137" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" s="138">
+        <v>6.0</v>
+      </c>
       <c r="G53" s="86"/>
-      <c r="H53" s="132"/>
+      <c r="H53" s="139"/>
       <c r="I53" s="86"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -3301,13 +3418,17 @@
     </row>
     <row r="54">
       <c r="A54" s="74"/>
-      <c r="B54" s="95"/>
+      <c r="B54" s="136" t="s">
+        <v>29</v>
+      </c>
       <c r="C54" s="94"/>
       <c r="D54" s="83"/>
-      <c r="E54" s="133"/>
-      <c r="F54" s="132"/>
+      <c r="E54" s="140" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="139"/>
       <c r="G54" s="86"/>
-      <c r="H54" s="132"/>
+      <c r="H54" s="139"/>
       <c r="I54" s="86"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -3338,22 +3459,28 @@
     </row>
     <row r="55">
       <c r="A55" s="74"/>
-      <c r="B55" s="96"/>
-      <c r="C55" s="134"/>
+      <c r="B55" s="141" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" s="142"/>
       <c r="D55" s="98"/>
-      <c r="E55" s="135"/>
-      <c r="F55" s="136"/>
+      <c r="E55" s="143" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" s="144">
+        <v>2.0</v>
+      </c>
       <c r="G55" s="101"/>
-      <c r="H55" s="136"/>
+      <c r="H55" s="145"/>
       <c r="I55" s="101"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
-      <c r="M55" s="137"/>
-      <c r="N55" s="137"/>
-      <c r="O55" s="137"/>
-      <c r="P55" s="137"/>
-      <c r="Q55" s="137">
+      <c r="M55" s="146"/>
+      <c r="N55" s="146"/>
+      <c r="O55" s="146"/>
+      <c r="P55" s="146"/>
+      <c r="Q55" s="146">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3375,14 +3502,18 @@
     </row>
     <row r="56">
       <c r="A56" s="74"/>
-      <c r="B56" s="54"/>
+      <c r="B56" s="32" t="s">
+        <v>44</v>
+      </c>
       <c r="C56" s="108"/>
       <c r="D56" s="76"/>
-      <c r="E56" s="122"/>
+      <c r="E56" s="147" t="s">
+        <v>16</v>
+      </c>
       <c r="F56" s="105"/>
       <c r="G56" s="109">
         <f>SUM(F57:F61)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H56" s="105"/>
       <c r="I56" s="109">
@@ -3418,13 +3549,19 @@
     </row>
     <row r="57">
       <c r="A57" s="74"/>
-      <c r="B57" s="95"/>
+      <c r="B57" s="148" t="s">
+        <v>36</v>
+      </c>
       <c r="C57" s="94"/>
       <c r="D57" s="83"/>
-      <c r="E57" s="133"/>
-      <c r="F57" s="132"/>
+      <c r="E57" s="149" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" s="138">
+        <v>2.0</v>
+      </c>
       <c r="G57" s="86"/>
-      <c r="H57" s="132"/>
+      <c r="H57" s="139"/>
       <c r="I57" s="86"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -3455,13 +3592,19 @@
     </row>
     <row r="58">
       <c r="A58" s="74"/>
-      <c r="B58" s="95"/>
+      <c r="B58" s="148" t="s">
+        <v>37</v>
+      </c>
       <c r="C58" s="94"/>
       <c r="D58" s="83"/>
-      <c r="E58" s="133"/>
-      <c r="F58" s="132"/>
+      <c r="E58" s="149" t="s">
+        <v>5</v>
+      </c>
+      <c r="F58" s="138">
+        <v>4.0</v>
+      </c>
       <c r="G58" s="86"/>
-      <c r="H58" s="132"/>
+      <c r="H58" s="139"/>
       <c r="I58" s="86"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -3492,13 +3635,19 @@
     </row>
     <row r="59">
       <c r="A59" s="74"/>
-      <c r="B59" s="95"/>
+      <c r="B59" s="136" t="s">
+        <v>45</v>
+      </c>
       <c r="C59" s="94"/>
       <c r="D59" s="83"/>
-      <c r="E59" s="133"/>
-      <c r="F59" s="132"/>
+      <c r="E59" s="149" t="s">
+        <v>5</v>
+      </c>
+      <c r="F59" s="138">
+        <v>4.0</v>
+      </c>
       <c r="G59" s="86"/>
-      <c r="H59" s="132"/>
+      <c r="H59" s="139"/>
       <c r="I59" s="86"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -3532,10 +3681,10 @@
       <c r="B60" s="95"/>
       <c r="C60" s="94"/>
       <c r="D60" s="83"/>
-      <c r="E60" s="133"/>
-      <c r="F60" s="132"/>
+      <c r="E60" s="150"/>
+      <c r="F60" s="139"/>
       <c r="G60" s="86"/>
-      <c r="H60" s="132"/>
+      <c r="H60" s="139"/>
       <c r="I60" s="86"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -3567,21 +3716,21 @@
     <row r="61">
       <c r="A61" s="74"/>
       <c r="B61" s="96"/>
-      <c r="C61" s="134"/>
+      <c r="C61" s="142"/>
       <c r="D61" s="98"/>
-      <c r="E61" s="135"/>
-      <c r="F61" s="136"/>
+      <c r="E61" s="151"/>
+      <c r="F61" s="145"/>
       <c r="G61" s="101"/>
-      <c r="H61" s="136"/>
+      <c r="H61" s="145"/>
       <c r="I61" s="101"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
-      <c r="M61" s="137"/>
-      <c r="N61" s="137"/>
-      <c r="O61" s="137"/>
-      <c r="P61" s="137"/>
-      <c r="Q61" s="137">
+      <c r="M61" s="146"/>
+      <c r="N61" s="146"/>
+      <c r="O61" s="146"/>
+      <c r="P61" s="146"/>
+      <c r="Q61" s="146">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3606,25 +3755,25 @@
       <c r="B62" s="11"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
-      <c r="E62" s="138"/>
-      <c r="F62" s="139"/>
-      <c r="G62" s="140">
+      <c r="E62" s="152"/>
+      <c r="F62" s="153"/>
+      <c r="G62" s="154">
         <f>SUM(F63:F64)</f>
         <v>0</v>
       </c>
-      <c r="H62" s="139"/>
-      <c r="I62" s="140">
+      <c r="H62" s="153"/>
+      <c r="I62" s="154">
         <f>SUM(H63:H64)</f>
         <v>0</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
-      <c r="M62" s="141"/>
-      <c r="N62" s="141"/>
-      <c r="O62" s="141"/>
-      <c r="P62" s="141"/>
-      <c r="Q62" s="141">
+      <c r="M62" s="155"/>
+      <c r="N62" s="155"/>
+      <c r="O62" s="155"/>
+      <c r="P62" s="155"/>
+      <c r="Q62" s="155">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3645,23 +3794,23 @@
       <c r="AF62" s="4"/>
     </row>
     <row r="63">
-      <c r="A63" s="124"/>
-      <c r="B63" s="125"/>
+      <c r="A63" s="129"/>
+      <c r="B63" s="156"/>
       <c r="C63" s="66"/>
       <c r="D63" s="67"/>
-      <c r="E63" s="142"/>
-      <c r="F63" s="143"/>
-      <c r="G63" s="128"/>
-      <c r="H63" s="143"/>
-      <c r="I63" s="129"/>
+      <c r="E63" s="157"/>
+      <c r="F63" s="158"/>
+      <c r="G63" s="133"/>
+      <c r="H63" s="158"/>
+      <c r="I63" s="134"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="130"/>
-      <c r="N63" s="130"/>
-      <c r="O63" s="130"/>
-      <c r="P63" s="130"/>
-      <c r="Q63" s="130">
+      <c r="M63" s="135"/>
+      <c r="N63" s="135"/>
+      <c r="O63" s="135"/>
+      <c r="P63" s="135"/>
+      <c r="Q63" s="135">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3682,23 +3831,23 @@
       <c r="AF63" s="4"/>
     </row>
     <row r="64">
-      <c r="A64" s="144"/>
+      <c r="A64" s="159"/>
       <c r="B64" s="96"/>
-      <c r="C64" s="134"/>
+      <c r="C64" s="142"/>
       <c r="D64" s="98"/>
-      <c r="E64" s="145"/>
-      <c r="F64" s="136"/>
+      <c r="E64" s="160"/>
+      <c r="F64" s="145"/>
       <c r="G64" s="101"/>
-      <c r="H64" s="136"/>
+      <c r="H64" s="145"/>
       <c r="I64" s="101"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
-      <c r="M64" s="137"/>
-      <c r="N64" s="137"/>
-      <c r="O64" s="137"/>
-      <c r="P64" s="137"/>
-      <c r="Q64" s="137">
+      <c r="M64" s="146"/>
+      <c r="N64" s="146"/>
+      <c r="O64" s="146"/>
+      <c r="P64" s="146"/>
+      <c r="Q64" s="146">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3719,73 +3868,73 @@
       <c r="AF64" s="4"/>
     </row>
     <row r="65">
-      <c r="A65" s="146" t="s">
+      <c r="A65" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="146"/>
-      <c r="C65" s="147"/>
-      <c r="D65" s="147"/>
-      <c r="E65" s="148"/>
-      <c r="F65" s="149">
+      <c r="B65" s="161"/>
+      <c r="C65" s="162"/>
+      <c r="D65" s="162"/>
+      <c r="E65" s="163"/>
+      <c r="F65" s="164">
         <f t="shared" ref="F65:G65" si="2">SUM(F5:F64)</f>
-        <v>42</v>
+        <v>69</v>
       </c>
-      <c r="G65" s="150">
+      <c r="G65" s="165">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>47</v>
       </c>
-      <c r="H65" s="151">
+      <c r="H65" s="166">
         <f>SUM(M65:P65)</f>
-        <v>59</v>
+        <v>77</v>
       </c>
-      <c r="I65" s="150">
+      <c r="I65" s="165">
         <f>SUM(I5:I64)</f>
         <v>10</v>
       </c>
-      <c r="J65" s="152"/>
-      <c r="K65" s="152"/>
-      <c r="L65" s="152"/>
-      <c r="M65" s="151">
+      <c r="J65" s="167"/>
+      <c r="K65" s="167"/>
+      <c r="L65" s="167"/>
+      <c r="M65" s="166">
         <f t="shared" ref="M65:P65" si="3">SUM(M5:M64)</f>
         <v>14</v>
       </c>
-      <c r="N65" s="151">
+      <c r="N65" s="166">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="O65" s="151">
+      <c r="O65" s="166">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="P65" s="151">
+      <c r="P65" s="166">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>33</v>
       </c>
-      <c r="Q65" s="151">
+      <c r="Q65" s="166">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>77</v>
       </c>
-      <c r="R65" s="152"/>
-      <c r="S65" s="152"/>
-      <c r="T65" s="152"/>
-      <c r="U65" s="152"/>
-      <c r="V65" s="152"/>
-      <c r="W65" s="152"/>
-      <c r="X65" s="152"/>
-      <c r="Y65" s="152"/>
-      <c r="Z65" s="152"/>
-      <c r="AA65" s="152"/>
-      <c r="AB65" s="152"/>
-      <c r="AC65" s="152"/>
-      <c r="AD65" s="152"/>
-      <c r="AE65" s="152"/>
-      <c r="AF65" s="152"/>
+      <c r="R65" s="167"/>
+      <c r="S65" s="167"/>
+      <c r="T65" s="167"/>
+      <c r="U65" s="167"/>
+      <c r="V65" s="167"/>
+      <c r="W65" s="167"/>
+      <c r="X65" s="167"/>
+      <c r="Y65" s="167"/>
+      <c r="Z65" s="167"/>
+      <c r="AA65" s="167"/>
+      <c r="AB65" s="167"/>
+      <c r="AC65" s="167"/>
+      <c r="AD65" s="167"/>
+      <c r="AE65" s="167"/>
+      <c r="AF65" s="167"/>
     </row>
     <row r="66">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
-      <c r="D66" s="153"/>
+      <c r="D66" s="168"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
@@ -3819,7 +3968,7 @@
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
-      <c r="D67" s="153"/>
+      <c r="D67" s="168"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
@@ -3853,7 +4002,7 @@
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="153"/>
+      <c r="D68" s="168"/>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>

</xml_diff>